<commit_message>
Added many inputs and To Do list.
Added efficiency choices to Fuel spreadsheet.
</commit_message>
<xml_diff>
--- a/heatpump/data/Fuel.xlsx
+++ b/heatpump/data/Fuel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CB21A7AF-23D9-490B-86AF-D6C25503BE9F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>btus</t>
   </si>
@@ -111,13 +112,40 @@
     <t>price_col</t>
   </si>
   <si>
-    <t>effic</t>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>effic_choices</t>
+  </si>
+  <si>
+    <t>[('Electric Resistance', 100)]</t>
+  </si>
+  <si>
+    <t>[('Standard', 80), ('High Efficiency Condensing', 95)]</t>
+  </si>
+  <si>
+    <t>[('Standard', 99)]</t>
+  </si>
+  <si>
+    <t>[('Standard', 80), ('High Efficiency (e.g. Toyostove)', 86)]</t>
+  </si>
+  <si>
+    <t>[('Standard', 80), ('High Efficiency', 86)]</t>
+  </si>
+  <si>
+    <t>[('Standard', 60), ('Catalytic', 70), ('Pellet', 75)]</t>
+  </si>
+  <si>
+    <t>[('Standard', 60)]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -533,11 +561,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,8 +574,9 @@
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.5703125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -567,11 +596,11 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>29</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,22 +608,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6">
-        <v>103700</v>
-      </c>
-      <c r="E2" s="5">
-        <v>117</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>3413</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="G2" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -602,22 +626,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6">
-        <v>91333</v>
+        <v>103700</v>
       </c>
       <c r="E3" s="5">
-        <v>139</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>117</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -625,22 +649,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6">
-        <v>137452</v>
+        <v>91333</v>
       </c>
       <c r="E4" s="5">
-        <v>161.30000000000001</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>139</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -648,22 +672,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="6">
-        <v>138500</v>
+        <v>137452</v>
       </c>
       <c r="E5" s="5">
         <v>161.30000000000001</v>
       </c>
-      <c r="F5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -671,22 +695,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="6">
-        <v>26200000</v>
+        <v>138500</v>
       </c>
       <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.63</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>161.30000000000001</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -694,22 +718,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="6">
-        <v>18100000</v>
+        <v>26200000</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7" s="8">
-        <v>0.63</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -717,22 +741,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6">
-        <v>15100000</v>
+        <v>18100000</v>
       </c>
       <c r="E8" s="5">
-        <v>214.3</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.63</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,22 +764,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6">
-        <v>960000</v>
+        <v>15100000</v>
       </c>
       <c r="E9" s="5">
-        <v>58</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.99</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>214.3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -763,22 +787,45 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6">
-        <v>1000000</v>
+        <v>960000</v>
       </c>
       <c r="E10" s="5">
         <v>58</v>
       </c>
-      <c r="F10" s="8">
-        <v>0.99</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="E11" s="5">
+        <v>58</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More output work.  Changed Oil Htg Effic. choices.
Table CSS changes to tighten padding.
</commit_message>
<xml_diff>
--- a/heatpump/data/Fuel.xlsx
+++ b/heatpump/data/Fuel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21015"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EE44EAC-17B5-4CD4-9630-3031D51AC9A6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A68F59A-60C9-41BB-91E9-954A54494DBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,16 @@
     </comment>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{6A6C571C-E425-4700-88B5-A57149765663}">
       <text>
-        <t>This is a typical DHW efficiency for the fuel type and is only used to back out DHW consumption from the user's entry of total fuel use if they state that the total includes DHW.</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This is a typical DHW efficiency for the fuel type and is only used to back out DHW consumption from the user's entry of total fuel use if they state that the total includes DHW.</t>
+        </r>
       </text>
     </comment>
     <comment ref="E11" authorId="0" shapeId="0" xr:uid="{34A63234-EFCA-4DBB-A329-952A37FEEBE8}">
@@ -115,7 +124,7 @@
     <t>GasPrice</t>
   </si>
   <si>
-    <t>[('Low 73%', 73), ('Standard 80%', 80), ('High Efficiency Condensing 95%', 95)]</t>
+    <t>[('Low 74%', 74), ('Standard 80%', 80), ('High Efficiency Condensing 95%', 95)]</t>
   </si>
   <si>
     <t>Propane</t>
@@ -133,7 +142,7 @@
     <t>Oil1Price</t>
   </si>
   <si>
-    <t>[('Low 73%', 73), ('Standard 80%', 80), ('High Efficiency (e.g. Toyostove) 86%', 86)]</t>
+    <t>[('Low 74%', 74), ('Standard 80%', 80), ('High Efficiency (e.g. Toyostove) 84%', 84)]</t>
   </si>
   <si>
     <t>#2 Oil</t>
@@ -142,7 +151,7 @@
     <t>Oil2Price</t>
   </si>
   <si>
-    <t>[('Low 73%', 73), ('Standard 80%', 80), ('High Efficiency 86%', 86)]</t>
+    <t>[('Low 74%', 74), ('Standard 80%', 80), ('High Efficiency 84%', 84)]</t>
   </si>
   <si>
     <t>Birch Wood</t>
@@ -626,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
More output.  Included Incremental Electricity Cost.
</commit_message>
<xml_diff>
--- a/heatpump/data/Fuel.xlsx
+++ b/heatpump/data/Fuel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A68F59A-60C9-41BB-91E9-954A54494DBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8082F8B3-1960-4ED4-B9D0-4F7E5E7FCE05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,7 +130,7 @@
     <t>Propane</t>
   </si>
   <si>
-    <t>gallons</t>
+    <t>gallon</t>
   </si>
   <si>
     <t>PropanePrice</t>
@@ -157,7 +157,7 @@
     <t>Birch Wood</t>
   </si>
   <si>
-    <t>cords</t>
+    <t>cord</t>
   </si>
   <si>
     <t>BirchPrice</t>
@@ -175,7 +175,7 @@
     <t>Wood Pellets</t>
   </si>
   <si>
-    <t>tons</t>
+    <t>ton</t>
   </si>
   <si>
     <t>WoodPelletsPrice</t>
@@ -208,7 +208,7 @@
     <t>District Heat, Hot Water</t>
   </si>
   <si>
-    <t>million BTU</t>
+    <t>million BTUs</t>
   </si>
   <si>
     <t>HotWaterPrice</t>
@@ -636,7 +636,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Calculations done for displacing Electric Heat.
Still need interface work and results reporting.
</commit_message>
<xml_diff>
--- a/heatpump/data/Fuel.xlsx
+++ b/heatpump/data/Fuel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21030"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8082F8B3-1960-4ED4-B9D0-4F7E5E7FCE05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23D2C398-E47C-4F2D-B1D4-765BD5D1B92F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -636,7 +636,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,7 +690,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="G2" s="7">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Hid proper Inputs for Electric Heat.
</commit_message>
<xml_diff>
--- a/heatpump/data/Fuel.xlsx
+++ b/heatpump/data/Fuel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23D2C398-E47C-4F2D-B1D4-765BD5D1B92F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2EBE713-E3A3-499D-BD39-7355DCEA6417}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
     <t>kWh</t>
   </si>
   <si>
-    <t>[('Electric Resistance', 100)]</t>
+    <t>[('Electric Resistance 100%', 100)]</t>
   </si>
   <si>
     <t>Natural Gas</t>
@@ -636,7 +636,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Changed Heat content of Birch and Coal according to AK Coop Extension page.
http://www.alaskawoodheating.com/energy_content.php
</commit_message>
<xml_diff>
--- a/heatpump/data/Fuel.xlsx
+++ b/heatpump/data/Fuel.xlsx
@@ -1,82 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21030"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2EBE713-E3A3-499D-BD39-7355DCEA6417}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="179020"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Alan Mitchell</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{785521D1-B934-48C4-89C7-3B0BACB91E14}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">This is pounds of CO2 per MMBtu.  See this page for the values below:  https://www.eia.gov/environment/emissions/co2_vol_mass.php
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{6A6C571C-E425-4700-88B5-A57149765663}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a typical DHW efficiency for the fuel type and is only used to back out DHW consumption from the user's entry of total fuel use if they state that the total includes DHW.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{34A63234-EFCA-4DBB-A329-952A37FEEBE8}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Using 1/2 the CO2 content of gas.  This is sometimes coming from waste heat, so has little incremental CO2 content.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -217,13 +151,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,17 +166,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -255,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -268,45 +198,83 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="18">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -317,10 +285,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -355,108 +323,74 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,54 +414,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -537,7 +470,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -546,7 +479,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -555,7 +488,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -563,10 +496,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -595,7 +528,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -608,13 +541,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -632,333 +564,335 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="65.5703125" customWidth="1"/>
+    <col min="1" max="1" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="65.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="8">
         <v>3413</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="G2" s="7">
+      <c r="E2" s="9"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="10">
         <v>0.93</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="8">
         <v>103700</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="9">
         <v>117</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="10">
+        <v>0.58</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="8">
         <v>91333</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="9">
         <v>139</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="10">
+        <v>0.58</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="8">
         <v>137452</v>
       </c>
-      <c r="E5" s="4">
-        <v>161.30000000000001</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="9">
+        <v>161.3</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="10">
         <v>0.6</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="8">
         <v>138500</v>
       </c>
-      <c r="E6" s="4">
-        <v>161.30000000000001</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="9">
+        <v>161.3</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="10">
         <v>0.6</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5">
-        <v>26200000</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="8">
+        <v>23600000</v>
+      </c>
+      <c r="E7" s="9">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="10">
         <v>0.5</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="8">
         <v>18100000</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="9">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="10">
         <v>0.5</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="8">
         <v>16000000</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="9">
         <v>0</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="7">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="10">
+        <v>0.55</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="5">
-        <v>15100000</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D10" s="8">
+        <v>17400000</v>
+      </c>
+      <c r="E10" s="9">
         <v>210.2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="10">
         <v>0.5</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="8">
         <v>960000</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="9">
         <v>58</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="10">
         <v>0.94</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="8">
         <v>1000000</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="9">
         <v>58</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="10">
         <v>0.94</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="11" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>